<commit_message>
update model configuration + filtering of mountains in the geopackeges
</commit_message>
<xml_diff>
--- a/notebooks/assets/test/RF10_1.xlsx
+++ b/notebooks/assets/test/RF10_1.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.042</v>
+        <v>1.262</v>
       </c>
       <c r="C2" t="n">
-        <v>0.96</v>
+        <v>1.141</v>
       </c>
       <c r="D2" t="n">
-        <v>0.869</v>
+        <v>0.791</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>1.239</v>
+        <v>1.509</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.661</v>
+        <v>2.507</v>
       </c>
       <c r="C3" t="n">
-        <v>1.636</v>
+        <v>2.335</v>
       </c>
       <c r="D3" t="n">
-        <v>1.742</v>
+        <v>1.137</v>
       </c>
       <c r="E3" t="n">
-        <v>0.665</v>
+        <v>0.833</v>
       </c>
       <c r="F3" t="n">
-        <v>2.782</v>
+        <v>4.191</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.754</v>
+        <v>0.659</v>
       </c>
       <c r="C4" t="n">
-        <v>0.852</v>
+        <v>0.8</v>
       </c>
       <c r="D4" t="n">
-        <v>0.793</v>
+        <v>0.789</v>
       </c>
       <c r="E4" t="n">
-        <v>0.66</v>
+        <v>0.645</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9</v>
+        <v>0.856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>